<commit_message>
MER editado e dicionario de dados finalizado
</commit_message>
<xml_diff>
--- a/Banco de Dados/dicionario de dados.xlsx
+++ b/Banco de Dados/dicionario de dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Rafael\Desktop\frigologia\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83CE1F46-238F-4B6C-8218-C2A428D3DB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A649413E-4F24-401E-B7EA-409FB4C9751A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C29389A7-3B49-441F-8E76-E5F84DC6EBBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
   <si>
     <t>tabela</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Estabelecimento</t>
   </si>
   <si>
-    <t>Armazena dados Dos estabelecimentos</t>
-  </si>
-  <si>
     <t>idEstabelecimento</t>
   </si>
   <si>
@@ -112,13 +109,115 @@
   </si>
   <si>
     <t>char</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armazena dados dos usuarios </t>
+  </si>
+  <si>
+    <t>Armazena dados dos estabelecimentos</t>
+  </si>
+  <si>
+    <t>Contem uma fk relacionada a tabela estabelecimento</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>fkEstabelecimento</t>
+  </si>
+  <si>
+    <t>Email estabelecimento</t>
+  </si>
+  <si>
+    <t>Senha do usuario</t>
+  </si>
+  <si>
+    <t>fk</t>
+  </si>
+  <si>
+    <t>Chave estrangeira da tabela estabelecimento</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Armazena os dados do dos freezers</t>
+  </si>
+  <si>
+    <t>idFreezer</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>Tipo de freezers horizontal/verdical</t>
+  </si>
+  <si>
+    <t>tamanho em litros</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Armazena as dados dados gerados por cada sensor e relaciona com o freezer</t>
+  </si>
+  <si>
+    <t>Contem uma fk relacionada a tabela freezer</t>
+  </si>
+  <si>
+    <t>idSensor</t>
+  </si>
+  <si>
+    <t>fkFreezer</t>
+  </si>
+  <si>
+    <t>Chave estrangeira da tabela freezer</t>
+  </si>
+  <si>
+    <t>Armazena os dados gerados pelos sensores</t>
+  </si>
+  <si>
+    <t>Dados</t>
+  </si>
+  <si>
+    <t>Contem uma fk relacionada a tabela dados</t>
+  </si>
+  <si>
+    <t>idDados</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>fkSensor</t>
+  </si>
+  <si>
+    <t>armazena data e hora de quando o dado foi obtido</t>
+  </si>
+  <si>
+    <t>Chave estrangeira da tabela sensor</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>diaHora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +225,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +258,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -161,26 +273,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1236CA5D-C29B-4E27-A897-36AEF19CF0D0}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,159 +700,713 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5">
+        <v>40</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="5">
+        <v>40</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="5">
+        <v>10</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="5">
+        <v>10</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="5">
+        <v>5</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="16"/>
+      <c r="D47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="32">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>